<commit_message>
Updated WBS file. Added additional WBS details.
</commit_message>
<xml_diff>
--- a/WBS(WeatherBasedCareCall).xlsx
+++ b/WBS(WeatherBasedCareCall).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/611da27b56fc6690/바탕 화면/github/WeatherBasedCareCall/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{3AD5BE18-9A6C-4EB1-878C-712667A965CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{66058F42-B23C-4409-A0D3-69CEB51CAC32}"/>
+  <xr:revisionPtr revIDLastSave="111" documentId="13_ncr:1_{3AD5BE18-9A6C-4EB1-878C-712667A965CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{81DECB9E-8869-42CD-9159-D3E539DBDAA9}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="108">
   <si>
     <t>WBS(Work Breakdown Structure)</t>
   </si>
@@ -178,9 +178,6 @@
   </si>
   <si>
     <t>프로세스 플로우차트 다이어그램 제작</t>
-  </si>
-  <si>
-    <t>프로젝트 발표</t>
   </si>
   <si>
     <t>데이터 수집 및 전처리</t>
@@ -290,10 +287,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>데이터 정제 및 변환(ETL)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>실시간 데이터 스트리밍</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -302,10 +295,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>실시간 데이터 처리 로직 개발(Spark, Kafka)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Java 애플리케이션 초기 설정</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -314,10 +303,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>알람 조작을 통해 안부전화를 걸 수 있는 로직 개발</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>데이터 분석 및 시각화</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -391,6 +376,34 @@
   </si>
   <si>
     <t>2일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>프로젝트 정리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>데이터 정제 및 변환(ETL) 점검</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>실시간 데이터 처리 로직 개발 연결 및 점검(Spark, Kafka)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이메일로 알람을 전송하는 기능 개발</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -763,11 +776,23 @@
     <xf numFmtId="0" fontId="2" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -776,18 +801,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -805,6 +818,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1008,8 +1025,8 @@
   <dimension ref="A1:AW1031"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O9" sqref="O9"/>
+      <pane ySplit="4" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1026,118 +1043,118 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:49" ht="38.25" customHeight="1">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
-      <c r="N1" s="39"/>
-      <c r="O1" s="39"/>
-      <c r="P1" s="39"/>
-      <c r="Q1" s="39"/>
-      <c r="R1" s="39"/>
-      <c r="S1" s="39"/>
-      <c r="T1" s="39"/>
-      <c r="U1" s="39"/>
-      <c r="V1" s="39"/>
-      <c r="W1" s="39"/>
-      <c r="X1" s="39"/>
-      <c r="Y1" s="39"/>
-      <c r="Z1" s="39"/>
-      <c r="AA1" s="39"/>
-      <c r="AB1" s="39"/>
-      <c r="AC1" s="39"/>
-      <c r="AD1" s="39"/>
-      <c r="AE1" s="39"/>
-      <c r="AF1" s="39"/>
-      <c r="AG1" s="39"/>
-      <c r="AH1" s="39"/>
-      <c r="AI1" s="39"/>
-      <c r="AJ1" s="39"/>
-      <c r="AK1" s="39"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="43"/>
+      <c r="P1" s="43"/>
+      <c r="Q1" s="43"/>
+      <c r="R1" s="43"/>
+      <c r="S1" s="43"/>
+      <c r="T1" s="43"/>
+      <c r="U1" s="43"/>
+      <c r="V1" s="43"/>
+      <c r="W1" s="43"/>
+      <c r="X1" s="43"/>
+      <c r="Y1" s="43"/>
+      <c r="Z1" s="43"/>
+      <c r="AA1" s="43"/>
+      <c r="AB1" s="43"/>
+      <c r="AC1" s="43"/>
+      <c r="AD1" s="43"/>
+      <c r="AE1" s="43"/>
+      <c r="AF1" s="43"/>
+      <c r="AG1" s="43"/>
+      <c r="AH1" s="43"/>
+      <c r="AI1" s="43"/>
+      <c r="AJ1" s="43"/>
+      <c r="AK1" s="43"/>
     </row>
     <row r="2" spans="1:49" ht="26.25" customHeight="1">
       <c r="A2" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="B2" s="40" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40"/>
-      <c r="N2" s="40"/>
-      <c r="O2" s="40"/>
-      <c r="P2" s="40"/>
-      <c r="Q2" s="40"/>
-      <c r="R2" s="40"/>
-      <c r="S2" s="40"/>
-      <c r="T2" s="40"/>
-      <c r="U2" s="40"/>
-      <c r="V2" s="40"/>
-      <c r="W2" s="40"/>
-      <c r="X2" s="40"/>
-      <c r="Y2" s="40"/>
-      <c r="Z2" s="40"/>
-      <c r="AA2" s="40"/>
-      <c r="AB2" s="40"/>
-      <c r="AC2" s="40"/>
-      <c r="AD2" s="40"/>
-      <c r="AE2" s="40"/>
-      <c r="AF2" s="40"/>
-      <c r="AG2" s="40"/>
-      <c r="AH2" s="40"/>
-      <c r="AI2" s="40"/>
-      <c r="AJ2" s="40"/>
-      <c r="AK2" s="40"/>
-      <c r="AL2" s="40"/>
-      <c r="AM2" s="40"/>
-      <c r="AN2" s="40"/>
-      <c r="AO2" s="40"/>
-      <c r="AP2" s="40"/>
-      <c r="AQ2" s="40"/>
-      <c r="AR2" s="40"/>
-      <c r="AS2" s="40"/>
-      <c r="AT2" s="40"/>
-      <c r="AU2" s="40"/>
-      <c r="AV2" s="40"/>
-      <c r="AW2" s="40"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="44"/>
+      <c r="N2" s="44"/>
+      <c r="O2" s="44"/>
+      <c r="P2" s="44"/>
+      <c r="Q2" s="44"/>
+      <c r="R2" s="44"/>
+      <c r="S2" s="44"/>
+      <c r="T2" s="44"/>
+      <c r="U2" s="44"/>
+      <c r="V2" s="44"/>
+      <c r="W2" s="44"/>
+      <c r="X2" s="44"/>
+      <c r="Y2" s="44"/>
+      <c r="Z2" s="44"/>
+      <c r="AA2" s="44"/>
+      <c r="AB2" s="44"/>
+      <c r="AC2" s="44"/>
+      <c r="AD2" s="44"/>
+      <c r="AE2" s="44"/>
+      <c r="AF2" s="44"/>
+      <c r="AG2" s="44"/>
+      <c r="AH2" s="44"/>
+      <c r="AI2" s="44"/>
+      <c r="AJ2" s="44"/>
+      <c r="AK2" s="44"/>
+      <c r="AL2" s="44"/>
+      <c r="AM2" s="44"/>
+      <c r="AN2" s="44"/>
+      <c r="AO2" s="44"/>
+      <c r="AP2" s="44"/>
+      <c r="AQ2" s="44"/>
+      <c r="AR2" s="44"/>
+      <c r="AS2" s="44"/>
+      <c r="AT2" s="44"/>
+      <c r="AU2" s="44"/>
+      <c r="AV2" s="44"/>
+      <c r="AW2" s="44"/>
     </row>
     <row r="3" spans="1:49" ht="13.5" customHeight="1">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="D3" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="36" t="s">
+      <c r="E3" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="36" t="s">
+      <c r="F3" s="38" t="s">
         <v>7</v>
       </c>
       <c r="G3" s="8" t="s">
@@ -1234,49 +1251,49 @@
         <v>38</v>
       </c>
       <c r="AL3" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="AM3" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="AM3" s="9" t="s">
+      <c r="AN3" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="AN3" s="9" t="s">
+      <c r="AO3" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="AO3" s="9" t="s">
+      <c r="AP3" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="AP3" s="9" t="s">
+      <c r="AQ3" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="AQ3" s="9" t="s">
+      <c r="AR3" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="AR3" s="9" t="s">
+      <c r="AS3" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="AS3" s="9" t="s">
+      <c r="AT3" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="AT3" s="9" t="s">
+      <c r="AU3" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="AU3" s="9" t="s">
+      <c r="AV3" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="AV3" s="9" t="s">
+      <c r="AW3" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="AW3" s="9" t="s">
-        <v>63</v>
-      </c>
     </row>
     <row r="4" spans="1:49" ht="13.5" customHeight="1">
-      <c r="A4" s="37"/>
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
+      <c r="A4" s="39"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
       <c r="G4" s="8">
         <v>45185</v>
       </c>
@@ -1408,11 +1425,11 @@
       </c>
     </row>
     <row r="5" spans="1:49" ht="17.25" customHeight="1">
-      <c r="A5" s="41" t="s">
+      <c r="A5" s="36" t="s">
         <v>39</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C5" s="10">
         <v>0.1</v>
@@ -1471,16 +1488,22 @@
       <c r="AW5" s="14"/>
     </row>
     <row r="6" spans="1:49" ht="17.25" customHeight="1">
-      <c r="A6" s="42"/>
+      <c r="A6" s="37"/>
       <c r="B6" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C6" s="10">
         <v>0</v>
       </c>
-      <c r="D6" s="11"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
+      <c r="D6" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="E6" s="12">
+        <v>45219</v>
+      </c>
+      <c r="F6" s="12">
+        <v>45219</v>
+      </c>
       <c r="G6" s="13"/>
       <c r="H6" s="13"/>
       <c r="I6" s="13"/>
@@ -1526,16 +1549,22 @@
       <c r="AW6" s="14"/>
     </row>
     <row r="7" spans="1:49" ht="17.25" customHeight="1">
-      <c r="A7" s="42"/>
+      <c r="A7" s="37"/>
       <c r="B7" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C7" s="10">
         <v>0</v>
       </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
+      <c r="D7" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="E7" s="12">
+        <v>45229</v>
+      </c>
+      <c r="F7" s="12">
+        <v>45229</v>
+      </c>
       <c r="G7" s="13"/>
       <c r="H7" s="13"/>
       <c r="I7" s="13"/>
@@ -1581,7 +1610,7 @@
       <c r="AW7" s="14"/>
     </row>
     <row r="8" spans="1:49" ht="17.25" customHeight="1">
-      <c r="A8" s="42"/>
+      <c r="A8" s="37"/>
       <c r="B8" s="15" t="s">
         <v>40</v>
       </c>
@@ -1637,15 +1666,15 @@
       <c r="AW8" s="14"/>
     </row>
     <row r="9" spans="1:49" ht="17.25" customHeight="1">
-      <c r="A9" s="42"/>
+      <c r="A9" s="37"/>
       <c r="B9" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C9" s="10">
         <v>0</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E9" s="12">
         <v>45195</v>
@@ -1698,16 +1727,22 @@
       <c r="AW9" s="14"/>
     </row>
     <row r="10" spans="1:49" ht="17.25" customHeight="1">
-      <c r="A10" s="42"/>
+      <c r="A10" s="37"/>
       <c r="B10" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C10" s="10">
         <v>0</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
+      <c r="D10" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="E10" s="12">
+        <v>45194</v>
+      </c>
+      <c r="F10" s="12">
+        <v>45198</v>
+      </c>
       <c r="G10" s="13"/>
       <c r="H10" s="13"/>
       <c r="I10" s="13"/>
@@ -1753,16 +1788,22 @@
       <c r="AW10" s="14"/>
     </row>
     <row r="11" spans="1:49" ht="17.25" customHeight="1">
-      <c r="A11" s="42"/>
+      <c r="A11" s="37"/>
       <c r="B11" s="3" t="s">
         <v>41</v>
       </c>
       <c r="C11" s="10">
         <v>0</v>
       </c>
-      <c r="D11" s="11"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
+      <c r="D11" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="E11" s="12">
+        <v>45196</v>
+      </c>
+      <c r="F11" s="12">
+        <v>45196</v>
+      </c>
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
       <c r="I11" s="13"/>
@@ -1808,7 +1849,7 @@
       <c r="AW11" s="14"/>
     </row>
     <row r="12" spans="1:49" ht="17.25" customHeight="1">
-      <c r="A12" s="42"/>
+      <c r="A12" s="37"/>
       <c r="B12" s="4" t="s">
         <v>42</v>
       </c>
@@ -1864,16 +1905,22 @@
       <c r="AW12" s="14"/>
     </row>
     <row r="13" spans="1:49" ht="17.25" customHeight="1">
-      <c r="A13" s="42"/>
+      <c r="A13" s="37"/>
       <c r="B13" s="3" t="s">
         <v>43</v>
       </c>
       <c r="C13" s="10">
         <v>0</v>
       </c>
-      <c r="D13" s="11"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
+      <c r="D13" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="E13" s="12">
+        <v>45199</v>
+      </c>
+      <c r="F13" s="12">
+        <v>45200</v>
+      </c>
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
       <c r="I13" s="17"/>
@@ -1919,16 +1966,22 @@
       <c r="AW13" s="14"/>
     </row>
     <row r="14" spans="1:49" ht="17.25" customHeight="1">
-      <c r="A14" s="42"/>
+      <c r="A14" s="37"/>
       <c r="B14" s="3" t="s">
         <v>44</v>
       </c>
       <c r="C14" s="10">
         <v>0</v>
       </c>
-      <c r="D14" s="11"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
+      <c r="D14" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="E14" s="12">
+        <v>45200</v>
+      </c>
+      <c r="F14" s="12">
+        <v>45201</v>
+      </c>
       <c r="G14" s="13"/>
       <c r="H14" s="13"/>
       <c r="I14" s="17"/>
@@ -1974,16 +2027,22 @@
       <c r="AW14" s="14"/>
     </row>
     <row r="15" spans="1:49" ht="17.25" customHeight="1">
-      <c r="A15" s="42"/>
+      <c r="A15" s="37"/>
       <c r="B15" s="3" t="s">
         <v>45</v>
       </c>
       <c r="C15" s="10">
         <v>0</v>
       </c>
-      <c r="D15" s="11"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
+      <c r="D15" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="E15" s="12">
+        <v>45202</v>
+      </c>
+      <c r="F15" s="12">
+        <v>45202</v>
+      </c>
       <c r="G15" s="13"/>
       <c r="H15" s="13"/>
       <c r="I15" s="17"/>
@@ -2029,16 +2088,22 @@
       <c r="AW15" s="14"/>
     </row>
     <row r="16" spans="1:49" ht="17.25" customHeight="1">
-      <c r="A16" s="42"/>
+      <c r="A16" s="37"/>
       <c r="B16" s="3" t="s">
         <v>46</v>
       </c>
       <c r="C16" s="10">
         <v>0</v>
       </c>
-      <c r="D16" s="11"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
+      <c r="D16" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="E16" s="12">
+        <v>45203</v>
+      </c>
+      <c r="F16" s="12">
+        <v>45203</v>
+      </c>
       <c r="G16" s="13"/>
       <c r="H16" s="13"/>
       <c r="I16" s="17"/>
@@ -2084,16 +2149,22 @@
       <c r="AW16" s="14"/>
     </row>
     <row r="17" spans="1:49" ht="17.25" customHeight="1">
-      <c r="A17" s="42"/>
+      <c r="A17" s="37"/>
       <c r="B17" s="3" t="s">
         <v>47</v>
       </c>
       <c r="C17" s="10">
         <v>0</v>
       </c>
-      <c r="D17" s="11"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
+      <c r="D17" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="E17" s="12">
+        <v>45219</v>
+      </c>
+      <c r="F17" s="12">
+        <v>45219</v>
+      </c>
       <c r="G17" s="13"/>
       <c r="H17" s="13"/>
       <c r="I17" s="17"/>
@@ -2139,9 +2210,9 @@
       <c r="AW17" s="14"/>
     </row>
     <row r="18" spans="1:49" ht="17.25" customHeight="1">
-      <c r="A18" s="42"/>
+      <c r="A18" s="37"/>
       <c r="B18" s="15" t="s">
-        <v>48</v>
+        <v>103</v>
       </c>
       <c r="C18" s="16">
         <f>AVERAGE(C19:C19)</f>
@@ -2195,16 +2266,22 @@
       <c r="AW18" s="14"/>
     </row>
     <row r="19" spans="1:49" ht="17.25" customHeight="1">
-      <c r="A19" s="42"/>
+      <c r="A19" s="37"/>
       <c r="B19" s="18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C19" s="10">
         <v>0</v>
       </c>
-      <c r="D19" s="11"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
+      <c r="D19" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="E19" s="12">
+        <v>45229</v>
+      </c>
+      <c r="F19" s="12">
+        <v>45230</v>
+      </c>
       <c r="G19" s="13"/>
       <c r="H19" s="13"/>
       <c r="I19" s="13"/>
@@ -2250,9 +2327,9 @@
       <c r="AW19" s="14"/>
     </row>
     <row r="20" spans="1:49" ht="17.25" customHeight="1">
-      <c r="A20" s="43"/>
+      <c r="A20" s="40"/>
       <c r="B20" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C20" s="16">
         <f>AVERAGE(C21:C25)</f>
@@ -2306,16 +2383,22 @@
       <c r="AW20" s="14"/>
     </row>
     <row r="21" spans="1:49" ht="17.25" customHeight="1">
-      <c r="A21" s="44"/>
+      <c r="A21" s="41"/>
       <c r="B21" s="19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C21" s="10">
         <v>0</v>
       </c>
-      <c r="D21" s="11"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="20"/>
+      <c r="D21" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="E21" s="12">
+        <v>45204</v>
+      </c>
+      <c r="F21" s="20">
+        <v>45204</v>
+      </c>
       <c r="G21" s="13"/>
       <c r="H21" s="17"/>
       <c r="I21" s="13"/>
@@ -2361,16 +2444,22 @@
       <c r="AW21" s="14"/>
     </row>
     <row r="22" spans="1:49" ht="17.25" customHeight="1">
-      <c r="A22" s="44"/>
+      <c r="A22" s="41"/>
       <c r="B22" s="19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C22" s="10">
         <v>0</v>
       </c>
-      <c r="D22" s="11"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
+      <c r="D22" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="E22" s="12">
+        <v>45205</v>
+      </c>
+      <c r="F22" s="12">
+        <v>45206</v>
+      </c>
       <c r="G22" s="13"/>
       <c r="H22" s="17"/>
       <c r="I22" s="13"/>
@@ -2416,16 +2505,22 @@
       <c r="AW22" s="14"/>
     </row>
     <row r="23" spans="1:49" ht="17.25" customHeight="1">
-      <c r="A23" s="44"/>
+      <c r="A23" s="41"/>
       <c r="B23" s="19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C23" s="10">
         <v>0</v>
       </c>
-      <c r="D23" s="11"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
+      <c r="D23" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="E23" s="12">
+        <v>45207</v>
+      </c>
+      <c r="F23" s="12">
+        <v>45207</v>
+      </c>
       <c r="G23" s="13"/>
       <c r="H23" s="13"/>
       <c r="I23" s="13"/>
@@ -2471,16 +2566,22 @@
       <c r="AW23" s="14"/>
     </row>
     <row r="24" spans="1:49" ht="17.25" customHeight="1">
-      <c r="A24" s="44"/>
+      <c r="A24" s="41"/>
       <c r="B24" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C24" s="10">
         <v>0</v>
       </c>
-      <c r="D24" s="11"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
+      <c r="D24" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="E24" s="12">
+        <v>45208</v>
+      </c>
+      <c r="F24" s="12">
+        <v>45209</v>
+      </c>
       <c r="G24" s="13"/>
       <c r="H24" s="13"/>
       <c r="I24" s="13"/>
@@ -2526,14 +2627,16 @@
       <c r="AW24" s="14"/>
     </row>
     <row r="25" spans="1:49" ht="17.25" customHeight="1">
-      <c r="A25" s="44"/>
+      <c r="A25" s="41"/>
       <c r="B25" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C25" s="10">
         <v>0</v>
       </c>
-      <c r="D25" s="11"/>
+      <c r="D25" s="11" t="s">
+        <v>101</v>
+      </c>
       <c r="E25" s="12"/>
       <c r="F25" s="12"/>
       <c r="G25" s="13"/>
@@ -2581,9 +2684,9 @@
       <c r="AW25" s="14"/>
     </row>
     <row r="26" spans="1:49" ht="17.25" customHeight="1">
-      <c r="A26" s="44"/>
+      <c r="A26" s="41"/>
       <c r="B26" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C26" s="16">
         <f>AVERAGE(C27:C29)</f>
@@ -2637,16 +2740,22 @@
       <c r="AW26" s="14"/>
     </row>
     <row r="27" spans="1:49" ht="17.25" customHeight="1">
-      <c r="A27" s="44"/>
+      <c r="A27" s="41"/>
       <c r="B27" s="22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C27" s="10">
         <v>0</v>
       </c>
-      <c r="D27" s="11"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
+      <c r="D27" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="E27" s="12">
+        <v>45210</v>
+      </c>
+      <c r="F27" s="12">
+        <v>45210</v>
+      </c>
       <c r="G27" s="13"/>
       <c r="H27" s="13"/>
       <c r="I27" s="13"/>
@@ -2692,16 +2801,22 @@
       <c r="AW27" s="14"/>
     </row>
     <row r="28" spans="1:49" ht="17.25" customHeight="1">
-      <c r="A28" s="44"/>
+      <c r="A28" s="41"/>
       <c r="B28" s="22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C28" s="10">
         <v>0</v>
       </c>
-      <c r="D28" s="11"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
+      <c r="D28" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="E28" s="12">
+        <v>45211</v>
+      </c>
+      <c r="F28" s="12">
+        <v>45211</v>
+      </c>
       <c r="G28" s="13"/>
       <c r="H28" s="13"/>
       <c r="I28" s="13"/>
@@ -2747,16 +2862,22 @@
       <c r="AW28" s="14"/>
     </row>
     <row r="29" spans="1:49" ht="17.25" customHeight="1">
-      <c r="A29" s="44"/>
+      <c r="A29" s="41"/>
       <c r="B29" s="22" t="s">
-        <v>79</v>
+        <v>104</v>
       </c>
       <c r="C29" s="10">
         <v>0</v>
       </c>
-      <c r="D29" s="11"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="12"/>
+      <c r="D29" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="E29" s="12">
+        <v>45214</v>
+      </c>
+      <c r="F29" s="12">
+        <v>45214</v>
+      </c>
       <c r="G29" s="13"/>
       <c r="H29" s="13"/>
       <c r="I29" s="13"/>
@@ -2802,9 +2923,9 @@
       <c r="AW29" s="14"/>
     </row>
     <row r="30" spans="1:49" ht="17.25" customHeight="1">
-      <c r="A30" s="44"/>
+      <c r="A30" s="41"/>
       <c r="B30" s="23" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C30" s="24">
         <f>AVERAGE(C31:C33)</f>
@@ -2858,16 +2979,22 @@
       <c r="AW30" s="14"/>
     </row>
     <row r="31" spans="1:49" ht="17.25" customHeight="1">
-      <c r="A31" s="44"/>
+      <c r="A31" s="41"/>
       <c r="B31" s="22" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C31" s="10">
         <v>0</v>
       </c>
-      <c r="D31" s="11"/>
-      <c r="E31" s="12"/>
-      <c r="F31" s="12"/>
+      <c r="D31" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="E31" s="12">
+        <v>45212</v>
+      </c>
+      <c r="F31" s="12">
+        <v>45212</v>
+      </c>
       <c r="G31" s="13"/>
       <c r="H31" s="13"/>
       <c r="I31" s="13"/>
@@ -2913,16 +3040,22 @@
       <c r="AW31" s="14"/>
     </row>
     <row r="32" spans="1:49" ht="17.25" customHeight="1">
-      <c r="A32" s="44"/>
+      <c r="A32" s="41"/>
       <c r="B32" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C32" s="10">
         <v>0</v>
       </c>
-      <c r="D32" s="11"/>
-      <c r="E32" s="12"/>
-      <c r="F32" s="12"/>
+      <c r="D32" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="E32" s="12">
+        <v>45213</v>
+      </c>
+      <c r="F32" s="12">
+        <v>45213</v>
+      </c>
       <c r="G32" s="13"/>
       <c r="H32" s="13"/>
       <c r="I32" s="13"/>
@@ -2968,16 +3101,22 @@
       <c r="AW32" s="14"/>
     </row>
     <row r="33" spans="1:49" ht="17.25" customHeight="1">
-      <c r="A33" s="44"/>
+      <c r="A33" s="41"/>
       <c r="B33" s="26" t="s">
-        <v>82</v>
+        <v>106</v>
       </c>
       <c r="C33" s="10">
         <v>0</v>
       </c>
-      <c r="D33" s="11"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="12"/>
+      <c r="D33" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="E33" s="12">
+        <v>45214</v>
+      </c>
+      <c r="F33" s="12">
+        <v>45214</v>
+      </c>
       <c r="G33" s="13"/>
       <c r="H33" s="13"/>
       <c r="I33" s="13"/>
@@ -3023,9 +3162,9 @@
       <c r="AW33" s="14"/>
     </row>
     <row r="34" spans="1:49" ht="17.25" customHeight="1">
-      <c r="A34" s="44"/>
+      <c r="A34" s="41"/>
       <c r="B34" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C34" s="24">
         <f>AVERAGE(C35:C37)</f>
@@ -3079,16 +3218,22 @@
       <c r="AW34" s="14"/>
     </row>
     <row r="35" spans="1:49" ht="17.25" customHeight="1">
-      <c r="A35" s="44"/>
+      <c r="A35" s="41"/>
       <c r="B35" s="22" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C35" s="10">
         <v>0</v>
       </c>
-      <c r="D35" s="11"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="12"/>
+      <c r="D35" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="E35" s="12">
+        <v>45215</v>
+      </c>
+      <c r="F35" s="12">
+        <v>45219</v>
+      </c>
       <c r="G35" s="13"/>
       <c r="H35" s="13"/>
       <c r="I35" s="13"/>
@@ -3134,16 +3279,22 @@
       <c r="AW35" s="14"/>
     </row>
     <row r="36" spans="1:49" ht="17.25" customHeight="1">
-      <c r="A36" s="44"/>
+      <c r="A36" s="41"/>
       <c r="B36" s="27" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C36" s="10">
         <v>0</v>
       </c>
-      <c r="D36" s="11"/>
-      <c r="E36" s="12"/>
-      <c r="F36" s="12"/>
+      <c r="D36" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="E36" s="12">
+        <v>45220</v>
+      </c>
+      <c r="F36" s="12">
+        <v>45221</v>
+      </c>
       <c r="G36" s="13"/>
       <c r="H36" s="13"/>
       <c r="I36" s="13"/>
@@ -3189,16 +3340,22 @@
       <c r="AW36" s="14"/>
     </row>
     <row r="37" spans="1:49" ht="17.25" customHeight="1">
-      <c r="A37" s="44"/>
+      <c r="A37" s="41"/>
       <c r="B37" s="22" t="s">
-        <v>85</v>
+        <v>107</v>
       </c>
       <c r="C37" s="10">
         <v>0</v>
       </c>
-      <c r="D37" s="11"/>
-      <c r="E37" s="12"/>
-      <c r="F37" s="12"/>
+      <c r="D37" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="E37" s="12">
+        <v>45222</v>
+      </c>
+      <c r="F37" s="12">
+        <v>45223</v>
+      </c>
       <c r="G37" s="13"/>
       <c r="H37" s="13"/>
       <c r="I37" s="13"/>
@@ -3244,9 +3401,9 @@
       <c r="AW37" s="14"/>
     </row>
     <row r="38" spans="1:49" ht="17.25" customHeight="1">
-      <c r="A38" s="44"/>
+      <c r="A38" s="41"/>
       <c r="B38" s="23" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C38" s="24">
         <f>AVERAGE(C39:C43)</f>
@@ -3300,16 +3457,22 @@
       <c r="AW38" s="14"/>
     </row>
     <row r="39" spans="1:49" ht="17.25" customHeight="1">
-      <c r="A39" s="44"/>
+      <c r="A39" s="41"/>
       <c r="B39" s="28" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C39" s="10">
         <v>0</v>
       </c>
-      <c r="D39" s="11"/>
-      <c r="E39" s="12"/>
-      <c r="F39" s="12"/>
+      <c r="D39" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="E39" s="12">
+        <v>45224</v>
+      </c>
+      <c r="F39" s="12">
+        <v>45224</v>
+      </c>
       <c r="G39" s="13"/>
       <c r="H39" s="13"/>
       <c r="I39" s="13"/>
@@ -3355,16 +3518,22 @@
       <c r="AW39" s="14"/>
     </row>
     <row r="40" spans="1:49" ht="17.25" customHeight="1">
-      <c r="A40" s="44"/>
+      <c r="A40" s="41"/>
       <c r="B40" s="28" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C40" s="10">
         <v>0</v>
       </c>
-      <c r="D40" s="11"/>
-      <c r="E40" s="12"/>
-      <c r="F40" s="12"/>
+      <c r="D40" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="E40" s="12">
+        <v>45225</v>
+      </c>
+      <c r="F40" s="12">
+        <v>45225</v>
+      </c>
       <c r="G40" s="13"/>
       <c r="H40" s="13"/>
       <c r="I40" s="13"/>
@@ -3410,16 +3579,22 @@
       <c r="AW40" s="14"/>
     </row>
     <row r="41" spans="1:49" ht="17.25" customHeight="1">
-      <c r="A41" s="44"/>
+      <c r="A41" s="41"/>
       <c r="B41" s="28" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C41" s="10">
         <v>0</v>
       </c>
-      <c r="D41" s="11"/>
-      <c r="E41" s="12"/>
-      <c r="F41" s="12"/>
+      <c r="D41" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="E41" s="12">
+        <v>45225</v>
+      </c>
+      <c r="F41" s="12">
+        <v>45225</v>
+      </c>
       <c r="G41" s="13"/>
       <c r="H41" s="13"/>
       <c r="I41" s="13"/>
@@ -3465,16 +3640,22 @@
       <c r="AW41" s="14"/>
     </row>
     <row r="42" spans="1:49" ht="17.25" customHeight="1">
-      <c r="A42" s="44"/>
+      <c r="A42" s="41"/>
       <c r="B42" s="28" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C42" s="10">
         <v>0</v>
       </c>
-      <c r="D42" s="11"/>
-      <c r="E42" s="12"/>
-      <c r="F42" s="12"/>
+      <c r="D42" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="E42" s="12">
+        <v>45226</v>
+      </c>
+      <c r="F42" s="12">
+        <v>45226</v>
+      </c>
       <c r="G42" s="13"/>
       <c r="H42" s="13"/>
       <c r="I42" s="13"/>
@@ -3520,16 +3701,22 @@
       <c r="AW42" s="14"/>
     </row>
     <row r="43" spans="1:49" ht="17.25" customHeight="1">
-      <c r="A43" s="44"/>
+      <c r="A43" s="41"/>
       <c r="B43" s="28" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C43" s="10">
         <v>0</v>
       </c>
-      <c r="D43" s="11"/>
-      <c r="E43" s="12"/>
-      <c r="F43" s="12"/>
+      <c r="D43" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="E43" s="12">
+        <v>45226</v>
+      </c>
+      <c r="F43" s="12">
+        <v>45226</v>
+      </c>
       <c r="G43" s="13"/>
       <c r="H43" s="13"/>
       <c r="I43" s="13"/>
@@ -3575,9 +3762,9 @@
       <c r="AW43" s="14"/>
     </row>
     <row r="44" spans="1:49" ht="17.25" customHeight="1">
-      <c r="A44" s="44"/>
+      <c r="A44" s="41"/>
       <c r="B44" s="23" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C44" s="24">
         <f>AVERAGE(C45:C47)</f>
@@ -3631,15 +3818,17 @@
       <c r="AW44" s="14"/>
     </row>
     <row r="45" spans="1:49" ht="17.25" customHeight="1">
-      <c r="A45" s="44"/>
+      <c r="A45" s="41"/>
       <c r="B45" s="28" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C45" s="10">
         <v>0</v>
       </c>
       <c r="D45" s="11"/>
-      <c r="E45" s="12"/>
+      <c r="E45" s="12">
+        <v>45227</v>
+      </c>
       <c r="F45" s="12"/>
       <c r="G45" s="13"/>
       <c r="H45" s="13"/>
@@ -3686,9 +3875,9 @@
       <c r="AW45" s="14"/>
     </row>
     <row r="46" spans="1:49" ht="17.25" customHeight="1">
-      <c r="A46" s="44"/>
+      <c r="A46" s="41"/>
       <c r="B46" s="28" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C46" s="10">
         <v>0</v>
@@ -3741,9 +3930,9 @@
       <c r="AW46" s="14"/>
     </row>
     <row r="47" spans="1:49" ht="17.25" customHeight="1">
-      <c r="A47" s="44"/>
+      <c r="A47" s="41"/>
       <c r="B47" s="28" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C47" s="10">
         <v>0</v>
@@ -3796,9 +3985,9 @@
       <c r="AW47" s="14"/>
     </row>
     <row r="48" spans="1:49" ht="17.25" customHeight="1">
-      <c r="A48" s="44"/>
+      <c r="A48" s="41"/>
       <c r="B48" s="15" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C48" s="24">
         <f>AVERAGE(C49:C51)</f>
@@ -3852,9 +4041,9 @@
       <c r="AW48" s="14"/>
     </row>
     <row r="49" spans="1:49" ht="17.25" customHeight="1">
-      <c r="A49" s="44"/>
+      <c r="A49" s="41"/>
       <c r="B49" s="28" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C49" s="10">
         <v>0</v>
@@ -3906,9 +4095,9 @@
       <c r="AW49" s="14"/>
     </row>
     <row r="50" spans="1:49" ht="17.25" customHeight="1">
-      <c r="A50" s="44"/>
+      <c r="A50" s="41"/>
       <c r="B50" s="28" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C50" s="10">
         <v>0</v>
@@ -3960,9 +4149,9 @@
       <c r="AW50" s="14"/>
     </row>
     <row r="51" spans="1:49" ht="17.25" customHeight="1">
-      <c r="A51" s="44"/>
+      <c r="A51" s="41"/>
       <c r="B51" s="29" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C51" s="30">
         <v>0</v>
@@ -4015,9 +4204,9 @@
       <c r="AW51" s="14"/>
     </row>
     <row r="52" spans="1:49" ht="17.25" customHeight="1">
-      <c r="A52" s="44"/>
+      <c r="A52" s="41"/>
       <c r="B52" s="15" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C52" s="24">
         <f>AVERAGE(C53)</f>
@@ -4071,9 +4260,9 @@
       <c r="AW52" s="14"/>
     </row>
     <row r="53" spans="1:49" ht="17.25" customHeight="1">
-      <c r="A53" s="44"/>
+      <c r="A53" s="41"/>
       <c r="B53" s="29" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C53" s="30">
         <v>0</v>
@@ -4126,9 +4315,9 @@
       <c r="AW53" s="14"/>
     </row>
     <row r="54" spans="1:49" ht="17.25" customHeight="1">
-      <c r="A54" s="44"/>
+      <c r="A54" s="41"/>
       <c r="B54" s="29" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C54" s="30">
         <v>0</v>
@@ -4181,9 +4370,9 @@
       <c r="AW54" s="14"/>
     </row>
     <row r="55" spans="1:49" ht="17.25" customHeight="1">
-      <c r="A55" s="44"/>
+      <c r="A55" s="41"/>
       <c r="B55" s="29" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C55" s="30">
         <v>0</v>

</xml_diff>

<commit_message>
Make a overview of WBCC.
</commit_message>
<xml_diff>
--- a/WBS(WeatherBasedCareCall).xlsx
+++ b/WBS(WeatherBasedCareCall).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/611da27b56fc6690/바탕 화면/github/WeatherBasedCareCall/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="111" documentId="13_ncr:1_{3AD5BE18-9A6C-4EB1-878C-712667A965CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{81DECB9E-8869-42CD-9159-D3E539DBDAA9}"/>
+  <xr:revisionPtr revIDLastSave="115" documentId="13_ncr:1_{3AD5BE18-9A6C-4EB1-878C-712667A965CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FD1096BB-E5A1-4CA2-B304-A982201300CD}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="107">
   <si>
     <t>WBS(Work Breakdown Structure)</t>
   </si>
@@ -392,10 +392,6 @@
   </si>
   <si>
     <t>데이터 정제 및 변환(ETL) 점검</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5일</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -820,10 +816,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
@@ -1025,8 +1017,8 @@
   <dimension ref="A1:AW1031"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D54" sqref="D54"/>
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -2637,8 +2629,12 @@
       <c r="D25" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
+      <c r="E25" s="12">
+        <v>45215</v>
+      </c>
+      <c r="F25" s="12">
+        <v>45215</v>
+      </c>
       <c r="G25" s="13"/>
       <c r="H25" s="13"/>
       <c r="I25" s="13"/>
@@ -3103,7 +3099,7 @@
     <row r="33" spans="1:49" ht="17.25" customHeight="1">
       <c r="A33" s="41"/>
       <c r="B33" s="26" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C33" s="10">
         <v>0</v>
@@ -3226,10 +3222,10 @@
         <v>0</v>
       </c>
       <c r="D35" s="11" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E35" s="12">
-        <v>45215</v>
+        <v>45216</v>
       </c>
       <c r="F35" s="12">
         <v>45219</v>
@@ -3342,7 +3338,7 @@
     <row r="37" spans="1:49" ht="17.25" customHeight="1">
       <c r="A37" s="41"/>
       <c r="B37" s="22" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C37" s="10">
         <v>0</v>

</xml_diff>

<commit_message>
Rewrite overall document and record progress on WBS.
</commit_message>
<xml_diff>
--- a/WBS(WeatherBasedCareCall).xlsx
+++ b/WBS(WeatherBasedCareCall).xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/611da27b56fc6690/바탕 화면/github/WeatherBasedCareCall/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smart\OneDrive\바탕 화면\github\WeatherBasedCareCall\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="119" documentId="13_ncr:1_{3AD5BE18-9A6C-4EB1-878C-712667A965CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7821DABE-A24F-45D5-987D-C4A723A25E33}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49ADDC29-DF78-4898-96A3-2CE47D91BDA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -816,10 +816,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
@@ -1020,9 +1016,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AW1031"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A20" sqref="A20:A55"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U9" sqref="U9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1428,7 +1424,7 @@
         <v>73</v>
       </c>
       <c r="C5" s="10">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>14</v>
@@ -1612,7 +1608,7 @@
       </c>
       <c r="C8" s="16">
         <f>AVERAGE(C9:C11)</f>
-        <v>0.70000000000000007</v>
+        <v>1</v>
       </c>
       <c r="D8" s="11"/>
       <c r="E8" s="12"/>
@@ -1728,7 +1724,7 @@
         <v>64</v>
       </c>
       <c r="C10" s="10">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D10" s="11" t="s">
         <v>102</v>
@@ -1851,7 +1847,7 @@
       </c>
       <c r="C12" s="16">
         <f>AVERAGE(C13:C17)</f>
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="D12" s="11"/>
       <c r="E12" s="12"/>
@@ -1906,7 +1902,7 @@
         <v>43</v>
       </c>
       <c r="C13" s="10">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="D13" s="11" t="s">
         <v>100</v>

</xml_diff>

<commit_message>
Added integration with KMA (Korea Meteorological Administration) API to the WBS
</commit_message>
<xml_diff>
--- a/WBS(WeatherBasedCareCall).xlsx
+++ b/WBS(WeatherBasedCareCall).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smart\OneDrive\바탕 화면\github\WeatherBasedCareCall\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\art\Desktop\WeatherBasedCareCall\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49ADDC29-DF78-4898-96A3-2CE47D91BDA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C51F7A0D-67D4-4A25-8A95-62522EE4BB12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="108">
   <si>
     <t>WBS(Work Breakdown Structure)</t>
   </si>
@@ -343,10 +343,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>배포 및 문서화</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>배포 계획</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -359,10 +355,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>유지보수 및 업데이트</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>버그 수정</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -400,6 +392,18 @@
   </si>
   <si>
     <t>이메일로 알람을 전송하는 기능 개발</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>배포 및 문서화(미정)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>유지보수 및 업데이트(미정)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1017,21 +1021,21 @@
   <dimension ref="A1:AW1031"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U9" sqref="U9"/>
+      <pane ySplit="4" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="53.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" style="6" customWidth="1"/>
+    <col min="2" max="2" width="53.85546875" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.140625" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="10" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="15" width="5.109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="16" max="27" width="5.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="15" width="5.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="16" max="27" width="5.28515625" style="6" bestFit="1" customWidth="1"/>
     <col min="28" max="49" width="6" style="6" bestFit="1" customWidth="1"/>
-    <col min="50" max="16384" width="14.44140625" style="6"/>
+    <col min="50" max="16384" width="14.42578125" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:49" ht="38.25" customHeight="1">
@@ -1488,7 +1492,7 @@
         <v>0</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E6" s="12">
         <v>45219</v>
@@ -1527,7 +1531,7 @@
       <c r="AI6" s="13"/>
       <c r="AJ6" s="13"/>
       <c r="AK6" s="13"/>
-      <c r="AL6" s="14"/>
+      <c r="AL6" s="35"/>
       <c r="AM6" s="14"/>
       <c r="AN6" s="14"/>
       <c r="AO6" s="14"/>
@@ -1549,7 +1553,7 @@
         <v>0</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E7" s="12">
         <v>45229</v>
@@ -1598,7 +1602,7 @@
       <c r="AS7" s="14"/>
       <c r="AT7" s="14"/>
       <c r="AU7" s="14"/>
-      <c r="AV7" s="14"/>
+      <c r="AV7" s="35"/>
       <c r="AW7" s="14"/>
     </row>
     <row r="8" spans="1:49" ht="17.25" customHeight="1">
@@ -1666,7 +1670,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E9" s="12">
         <v>45195</v>
@@ -1727,7 +1731,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E10" s="12">
         <v>45194</v>
@@ -1741,11 +1745,11 @@
       <c r="J10" s="13"/>
       <c r="K10" s="13"/>
       <c r="L10" s="13"/>
-      <c r="M10" s="13"/>
-      <c r="N10" s="13"/>
-      <c r="O10" s="13"/>
-      <c r="P10" s="13"/>
-      <c r="Q10" s="13"/>
+      <c r="M10" s="35"/>
+      <c r="N10" s="35"/>
+      <c r="O10" s="35"/>
+      <c r="P10" s="35"/>
+      <c r="Q10" s="35"/>
       <c r="R10" s="13"/>
       <c r="S10" s="13"/>
       <c r="T10" s="13"/>
@@ -1788,7 +1792,7 @@
         <v>1</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E11" s="12">
         <v>45196</v>
@@ -1804,7 +1808,7 @@
       <c r="L11" s="13"/>
       <c r="M11" s="13"/>
       <c r="N11" s="13"/>
-      <c r="O11" s="13"/>
+      <c r="O11" s="35"/>
       <c r="P11" s="13"/>
       <c r="Q11" s="13"/>
       <c r="R11" s="13"/>
@@ -1847,7 +1851,7 @@
       </c>
       <c r="C12" s="16">
         <f>AVERAGE(C13:C17)</f>
-        <v>0.02</v>
+        <v>0.8</v>
       </c>
       <c r="D12" s="11"/>
       <c r="E12" s="12"/>
@@ -1902,10 +1906,10 @@
         <v>43</v>
       </c>
       <c r="C13" s="10">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E13" s="12">
         <v>45199</v>
@@ -1924,8 +1928,8 @@
       <c r="O13" s="13"/>
       <c r="P13" s="13"/>
       <c r="Q13" s="13"/>
-      <c r="R13" s="13"/>
-      <c r="S13" s="13"/>
+      <c r="R13" s="35"/>
+      <c r="S13" s="35"/>
       <c r="T13" s="13"/>
       <c r="U13" s="13"/>
       <c r="V13" s="13"/>
@@ -1963,10 +1967,10 @@
         <v>44</v>
       </c>
       <c r="C14" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E14" s="12">
         <v>45200</v>
@@ -1986,8 +1990,8 @@
       <c r="P14" s="13"/>
       <c r="Q14" s="13"/>
       <c r="R14" s="13"/>
-      <c r="S14" s="13"/>
-      <c r="T14" s="13"/>
+      <c r="S14" s="35"/>
+      <c r="T14" s="35"/>
       <c r="U14" s="13"/>
       <c r="V14" s="13"/>
       <c r="W14" s="13"/>
@@ -2024,10 +2028,10 @@
         <v>45</v>
       </c>
       <c r="C15" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E15" s="12">
         <v>45202</v>
@@ -2049,7 +2053,7 @@
       <c r="R15" s="13"/>
       <c r="S15" s="13"/>
       <c r="T15" s="13"/>
-      <c r="U15" s="13"/>
+      <c r="U15" s="35"/>
       <c r="V15" s="13"/>
       <c r="W15" s="13"/>
       <c r="X15" s="13"/>
@@ -2085,10 +2089,10 @@
         <v>46</v>
       </c>
       <c r="C16" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E16" s="12">
         <v>45203</v>
@@ -2111,7 +2115,7 @@
       <c r="S16" s="13"/>
       <c r="T16" s="13"/>
       <c r="U16" s="13"/>
-      <c r="V16" s="13"/>
+      <c r="V16" s="35"/>
       <c r="W16" s="13"/>
       <c r="X16" s="13"/>
       <c r="Y16" s="13"/>
@@ -2149,7 +2153,7 @@
         <v>0</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E17" s="12">
         <v>45219</v>
@@ -2188,7 +2192,7 @@
       <c r="AI17" s="13"/>
       <c r="AJ17" s="13"/>
       <c r="AK17" s="13"/>
-      <c r="AL17" s="14"/>
+      <c r="AL17" s="35"/>
       <c r="AM17" s="14"/>
       <c r="AN17" s="14"/>
       <c r="AO17" s="14"/>
@@ -2204,7 +2208,7 @@
     <row r="18" spans="1:49" ht="17.25" customHeight="1">
       <c r="A18" s="37"/>
       <c r="B18" s="15" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C18" s="16">
         <f>AVERAGE(C19:C19)</f>
@@ -2254,8 +2258,8 @@
       <c r="AS18" s="14"/>
       <c r="AT18" s="14"/>
       <c r="AU18" s="14"/>
-      <c r="AV18" s="14"/>
-      <c r="AW18" s="14"/>
+      <c r="AV18" s="35"/>
+      <c r="AW18" s="35"/>
     </row>
     <row r="19" spans="1:49" ht="17.25" customHeight="1">
       <c r="A19" s="37"/>
@@ -2266,7 +2270,7 @@
         <v>0</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E19" s="12">
         <v>45229</v>
@@ -2383,7 +2387,7 @@
         <v>0</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E21" s="12">
         <v>45204</v>
@@ -2407,7 +2411,7 @@
       <c r="T21" s="13"/>
       <c r="U21" s="13"/>
       <c r="V21" s="13"/>
-      <c r="W21" s="13"/>
+      <c r="W21" s="35"/>
       <c r="X21" s="13"/>
       <c r="Y21" s="13"/>
       <c r="Z21" s="13"/>
@@ -2444,7 +2448,7 @@
         <v>0</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E22" s="12">
         <v>45205</v>
@@ -2469,8 +2473,8 @@
       <c r="U22" s="13"/>
       <c r="V22" s="13"/>
       <c r="W22" s="13"/>
-      <c r="X22" s="13"/>
-      <c r="Y22" s="13"/>
+      <c r="X22" s="35"/>
+      <c r="Y22" s="35"/>
       <c r="Z22" s="13"/>
       <c r="AA22" s="13"/>
       <c r="AB22" s="13"/>
@@ -2505,7 +2509,7 @@
         <v>0</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E23" s="12">
         <v>45207</v>
@@ -2532,7 +2536,7 @@
       <c r="W23" s="13"/>
       <c r="X23" s="13"/>
       <c r="Y23" s="13"/>
-      <c r="Z23" s="13"/>
+      <c r="Z23" s="35"/>
       <c r="AA23" s="13"/>
       <c r="AB23" s="13"/>
       <c r="AC23" s="13"/>
@@ -2566,7 +2570,7 @@
         <v>0</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E24" s="12">
         <v>45208</v>
@@ -2594,8 +2598,8 @@
       <c r="X24" s="13"/>
       <c r="Y24" s="13"/>
       <c r="Z24" s="13"/>
-      <c r="AA24" s="13"/>
-      <c r="AB24" s="13"/>
+      <c r="AA24" s="35"/>
+      <c r="AB24" s="35"/>
       <c r="AC24" s="13"/>
       <c r="AD24" s="13"/>
       <c r="AE24" s="13"/>
@@ -2627,7 +2631,7 @@
         <v>0</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E25" s="12">
         <v>45215</v>
@@ -2662,7 +2666,7 @@
       <c r="AE25" s="13"/>
       <c r="AF25" s="13"/>
       <c r="AG25" s="13"/>
-      <c r="AH25" s="13"/>
+      <c r="AH25" s="35"/>
       <c r="AI25" s="13"/>
       <c r="AJ25" s="13"/>
       <c r="AK25" s="13"/>
@@ -2744,7 +2748,7 @@
         <v>0</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E27" s="12">
         <v>45210</v>
@@ -2774,7 +2778,7 @@
       <c r="Z27" s="13"/>
       <c r="AA27" s="13"/>
       <c r="AB27" s="13"/>
-      <c r="AC27" s="13"/>
+      <c r="AC27" s="35"/>
       <c r="AD27" s="13"/>
       <c r="AE27" s="13"/>
       <c r="AF27" s="13"/>
@@ -2805,7 +2809,7 @@
         <v>0</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E28" s="12">
         <v>45211</v>
@@ -2836,7 +2840,7 @@
       <c r="AA28" s="13"/>
       <c r="AB28" s="13"/>
       <c r="AC28" s="13"/>
-      <c r="AD28" s="13"/>
+      <c r="AD28" s="35"/>
       <c r="AE28" s="13"/>
       <c r="AF28" s="13"/>
       <c r="AG28" s="13"/>
@@ -2860,13 +2864,13 @@
     <row r="29" spans="1:49" ht="17.25" customHeight="1">
       <c r="A29" s="41"/>
       <c r="B29" s="22" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C29" s="10">
         <v>0</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E29" s="12">
         <v>45214</v>
@@ -2900,7 +2904,7 @@
       <c r="AD29" s="13"/>
       <c r="AE29" s="13"/>
       <c r="AF29" s="13"/>
-      <c r="AG29" s="13"/>
+      <c r="AG29" s="35"/>
       <c r="AH29" s="13"/>
       <c r="AI29" s="13"/>
       <c r="AJ29" s="13"/>
@@ -2983,7 +2987,7 @@
         <v>0</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E31" s="12">
         <v>45212</v>
@@ -3015,7 +3019,7 @@
       <c r="AB31" s="13"/>
       <c r="AC31" s="13"/>
       <c r="AD31" s="13"/>
-      <c r="AE31" s="13"/>
+      <c r="AE31" s="35"/>
       <c r="AF31" s="13"/>
       <c r="AG31" s="13"/>
       <c r="AH31" s="13"/>
@@ -3044,7 +3048,7 @@
         <v>0</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E32" s="12">
         <v>45213</v>
@@ -3077,7 +3081,7 @@
       <c r="AC32" s="13"/>
       <c r="AD32" s="13"/>
       <c r="AE32" s="13"/>
-      <c r="AF32" s="13"/>
+      <c r="AF32" s="35"/>
       <c r="AG32" s="13"/>
       <c r="AH32" s="13"/>
       <c r="AI32" s="13"/>
@@ -3099,13 +3103,13 @@
     <row r="33" spans="1:49" ht="17.25" customHeight="1">
       <c r="A33" s="41"/>
       <c r="B33" s="26" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C33" s="10">
         <v>0</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E33" s="12">
         <v>45214</v>
@@ -3139,7 +3143,7 @@
       <c r="AD33" s="13"/>
       <c r="AE33" s="13"/>
       <c r="AF33" s="13"/>
-      <c r="AG33" s="13"/>
+      <c r="AG33" s="35"/>
       <c r="AH33" s="13"/>
       <c r="AI33" s="13"/>
       <c r="AJ33" s="13"/>
@@ -3222,7 +3226,7 @@
         <v>0</v>
       </c>
       <c r="D35" s="11" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E35" s="12">
         <v>45216</v>
@@ -3258,10 +3262,10 @@
       <c r="AF35" s="13"/>
       <c r="AG35" s="13"/>
       <c r="AH35" s="13"/>
-      <c r="AI35" s="13"/>
-      <c r="AJ35" s="13"/>
-      <c r="AK35" s="13"/>
-      <c r="AL35" s="14"/>
+      <c r="AI35" s="35"/>
+      <c r="AJ35" s="35"/>
+      <c r="AK35" s="35"/>
+      <c r="AL35" s="35"/>
       <c r="AM35" s="14"/>
       <c r="AN35" s="14"/>
       <c r="AO35" s="14"/>
@@ -3283,7 +3287,7 @@
         <v>0</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E36" s="12">
         <v>45220</v>
@@ -3323,8 +3327,8 @@
       <c r="AJ36" s="13"/>
       <c r="AK36" s="13"/>
       <c r="AL36" s="14"/>
-      <c r="AM36" s="14"/>
-      <c r="AN36" s="14"/>
+      <c r="AM36" s="35"/>
+      <c r="AN36" s="35"/>
       <c r="AO36" s="14"/>
       <c r="AP36" s="14"/>
       <c r="AQ36" s="14"/>
@@ -3338,13 +3342,13 @@
     <row r="37" spans="1:49" ht="17.25" customHeight="1">
       <c r="A37" s="41"/>
       <c r="B37" s="22" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C37" s="10">
         <v>0</v>
       </c>
       <c r="D37" s="11" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E37" s="12">
         <v>45222</v>
@@ -3386,8 +3390,8 @@
       <c r="AL37" s="14"/>
       <c r="AM37" s="14"/>
       <c r="AN37" s="14"/>
-      <c r="AO37" s="14"/>
-      <c r="AP37" s="14"/>
+      <c r="AO37" s="35"/>
+      <c r="AP37" s="35"/>
       <c r="AQ37" s="14"/>
       <c r="AR37" s="14"/>
       <c r="AS37" s="14"/>
@@ -3461,7 +3465,7 @@
         <v>0</v>
       </c>
       <c r="D39" s="11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E39" s="12">
         <v>45224</v>
@@ -3505,7 +3509,7 @@
       <c r="AN39" s="14"/>
       <c r="AO39" s="14"/>
       <c r="AP39" s="14"/>
-      <c r="AQ39" s="14"/>
+      <c r="AQ39" s="35"/>
       <c r="AR39" s="14"/>
       <c r="AS39" s="14"/>
       <c r="AT39" s="14"/>
@@ -3522,7 +3526,7 @@
         <v>0</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E40" s="12">
         <v>45225</v>
@@ -3567,7 +3571,7 @@
       <c r="AO40" s="14"/>
       <c r="AP40" s="14"/>
       <c r="AQ40" s="14"/>
-      <c r="AR40" s="14"/>
+      <c r="AR40" s="35"/>
       <c r="AS40" s="14"/>
       <c r="AT40" s="14"/>
       <c r="AU40" s="14"/>
@@ -3583,7 +3587,7 @@
         <v>0</v>
       </c>
       <c r="D41" s="11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E41" s="12">
         <v>45225</v>
@@ -3628,7 +3632,7 @@
       <c r="AO41" s="14"/>
       <c r="AP41" s="14"/>
       <c r="AQ41" s="14"/>
-      <c r="AR41" s="14"/>
+      <c r="AR41" s="35"/>
       <c r="AS41" s="14"/>
       <c r="AT41" s="14"/>
       <c r="AU41" s="14"/>
@@ -3644,7 +3648,7 @@
         <v>0</v>
       </c>
       <c r="D42" s="11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E42" s="12">
         <v>45226</v>
@@ -3690,7 +3694,7 @@
       <c r="AP42" s="14"/>
       <c r="AQ42" s="14"/>
       <c r="AR42" s="14"/>
-      <c r="AS42" s="14"/>
+      <c r="AS42" s="35"/>
       <c r="AT42" s="14"/>
       <c r="AU42" s="14"/>
       <c r="AV42" s="14"/>
@@ -3705,7 +3709,7 @@
         <v>0</v>
       </c>
       <c r="D43" s="11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E43" s="12">
         <v>45226</v>
@@ -3751,7 +3755,7 @@
       <c r="AP43" s="14"/>
       <c r="AQ43" s="14"/>
       <c r="AR43" s="14"/>
-      <c r="AS43" s="14"/>
+      <c r="AS43" s="35"/>
       <c r="AT43" s="14"/>
       <c r="AU43" s="14"/>
       <c r="AV43" s="14"/>
@@ -3821,11 +3825,15 @@
       <c r="C45" s="10">
         <v>0</v>
       </c>
-      <c r="D45" s="11"/>
+      <c r="D45" s="11" t="s">
+        <v>99</v>
+      </c>
       <c r="E45" s="12">
         <v>45227</v>
       </c>
-      <c r="F45" s="12"/>
+      <c r="F45" s="12">
+        <v>45227</v>
+      </c>
       <c r="G45" s="13"/>
       <c r="H45" s="13"/>
       <c r="I45" s="13"/>
@@ -3865,7 +3873,7 @@
       <c r="AQ45" s="14"/>
       <c r="AR45" s="14"/>
       <c r="AS45" s="14"/>
-      <c r="AT45" s="14"/>
+      <c r="AT45" s="35"/>
       <c r="AU45" s="14"/>
       <c r="AV45" s="14"/>
       <c r="AW45" s="14"/>
@@ -3878,9 +3886,15 @@
       <c r="C46" s="10">
         <v>0</v>
       </c>
-      <c r="D46" s="11"/>
-      <c r="E46" s="12"/>
-      <c r="F46" s="12"/>
+      <c r="D46" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="E46" s="12">
+        <v>45227</v>
+      </c>
+      <c r="F46" s="12">
+        <v>45227</v>
+      </c>
       <c r="G46" s="13"/>
       <c r="H46" s="13"/>
       <c r="I46" s="13"/>
@@ -3920,7 +3934,7 @@
       <c r="AQ46" s="14"/>
       <c r="AR46" s="14"/>
       <c r="AS46" s="14"/>
-      <c r="AT46" s="14"/>
+      <c r="AT46" s="35"/>
       <c r="AU46" s="14"/>
       <c r="AV46" s="14"/>
       <c r="AW46" s="14"/>
@@ -3933,9 +3947,15 @@
       <c r="C47" s="10">
         <v>0</v>
       </c>
-      <c r="D47" s="11"/>
-      <c r="E47" s="12"/>
-      <c r="F47" s="12"/>
+      <c r="D47" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="E47" s="12">
+        <v>45227</v>
+      </c>
+      <c r="F47" s="12">
+        <v>45227</v>
+      </c>
       <c r="G47" s="13"/>
       <c r="H47" s="13"/>
       <c r="I47" s="13"/>
@@ -3975,7 +3995,7 @@
       <c r="AQ47" s="14"/>
       <c r="AR47" s="14"/>
       <c r="AS47" s="14"/>
-      <c r="AT47" s="14"/>
+      <c r="AT47" s="35"/>
       <c r="AU47" s="14"/>
       <c r="AV47" s="14"/>
       <c r="AW47" s="14"/>
@@ -3983,7 +4003,7 @@
     <row r="48" spans="1:49" ht="17.25" customHeight="1">
       <c r="A48" s="41"/>
       <c r="B48" s="15" t="s">
-        <v>92</v>
+        <v>106</v>
       </c>
       <c r="C48" s="24">
         <f>AVERAGE(C49:C51)</f>
@@ -4039,12 +4059,14 @@
     <row r="49" spans="1:49" ht="17.25" customHeight="1">
       <c r="A49" s="41"/>
       <c r="B49" s="28" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C49" s="10">
         <v>0</v>
       </c>
-      <c r="D49" s="11"/>
+      <c r="D49" s="11" t="s">
+        <v>105</v>
+      </c>
       <c r="E49" s="12"/>
       <c r="F49" s="12"/>
       <c r="G49" s="13"/>
@@ -4093,7 +4115,7 @@
     <row r="50" spans="1:49" ht="17.25" customHeight="1">
       <c r="A50" s="41"/>
       <c r="B50" s="28" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C50" s="10">
         <v>0</v>
@@ -4147,7 +4169,7 @@
     <row r="51" spans="1:49" ht="17.25" customHeight="1">
       <c r="A51" s="41"/>
       <c r="B51" s="29" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C51" s="30">
         <v>0</v>
@@ -4202,7 +4224,7 @@
     <row r="52" spans="1:49" ht="17.25" customHeight="1">
       <c r="A52" s="41"/>
       <c r="B52" s="15" t="s">
-        <v>96</v>
+        <v>107</v>
       </c>
       <c r="C52" s="24">
         <f>AVERAGE(C53)</f>
@@ -4258,7 +4280,7 @@
     <row r="53" spans="1:49" ht="17.25" customHeight="1">
       <c r="A53" s="41"/>
       <c r="B53" s="29" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C53" s="30">
         <v>0</v>
@@ -4313,7 +4335,7 @@
     <row r="54" spans="1:49" ht="17.25" customHeight="1">
       <c r="A54" s="41"/>
       <c r="B54" s="29" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C54" s="30">
         <v>0</v>
@@ -4368,7 +4390,7 @@
     <row r="55" spans="1:49" ht="17.25" customHeight="1">
       <c r="A55" s="41"/>
       <c r="B55" s="29" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C55" s="30">
         <v>0</v>

</xml_diff>

<commit_message>
Added integration to WBS about wrote code to gather weather data from the KMA API
</commit_message>
<xml_diff>
--- a/WBS(WeatherBasedCareCall).xlsx
+++ b/WBS(WeatherBasedCareCall).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\art\Desktop\WeatherBasedCareCall\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C51F7A0D-67D4-4A25-8A95-62522EE4BB12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B73C0EF2-C7B9-4939-BE57-102DE56627DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1021,8 +1021,8 @@
   <dimension ref="A1:AW1031"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B52" sqref="B52"/>
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2329,7 +2329,7 @@
       </c>
       <c r="C20" s="16">
         <f>AVERAGE(C21:C25)</f>
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="D20" s="11"/>
       <c r="E20" s="12"/>
@@ -2384,7 +2384,7 @@
         <v>65</v>
       </c>
       <c r="C21" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21" s="11" t="s">
         <v>99</v>
@@ -2445,7 +2445,7 @@
         <v>66</v>
       </c>
       <c r="C22" s="10">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="D22" s="11" t="s">
         <v>98</v>

</xml_diff>

<commit_message>
Wrote initial settings in hadoop at Hadoop 초기 설정.docx
</commit_message>
<xml_diff>
--- a/WBS(WeatherBasedCareCall).xlsx
+++ b/WBS(WeatherBasedCareCall).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\art\Desktop\WeatherBasedCareCall\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B73C0EF2-C7B9-4939-BE57-102DE56627DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D740CBC-FBE8-4288-AC17-2E05C5C699C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1022,7 +1022,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C22" sqref="C22"/>
+      <selection pane="bottomLeft" activeCell="Q36" sqref="Q36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2329,7 +2329,7 @@
       </c>
       <c r="C20" s="16">
         <f>AVERAGE(C21:C25)</f>
-        <v>0.3</v>
+        <v>0.6</v>
       </c>
       <c r="D20" s="11"/>
       <c r="E20" s="12"/>
@@ -2445,7 +2445,7 @@
         <v>66</v>
       </c>
       <c r="C22" s="10">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D22" s="11" t="s">
         <v>98</v>
@@ -2506,7 +2506,7 @@
         <v>75</v>
       </c>
       <c r="C23" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D23" s="11" t="s">
         <v>99</v>

</xml_diff>

<commit_message>
Organized folders and nearly completed partial data collection and storage logic.
</commit_message>
<xml_diff>
--- a/WBS(WeatherBasedCareCall).xlsx
+++ b/WBS(WeatherBasedCareCall).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\art\Desktop\WeatherBasedCareCall\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37F5F2C8-7AD5-4FC2-B38D-1A83D8AD81BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E310D08-609D-4167-A020-3E5710C2FC06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1022,7 +1022,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G21" sqref="G21"/>
+      <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2329,7 +2329,7 @@
       </c>
       <c r="C20" s="16">
         <f>AVERAGE(C21:C25)</f>
-        <v>0.62</v>
+        <v>0.74</v>
       </c>
       <c r="D20" s="11"/>
       <c r="E20" s="12"/>
@@ -2567,7 +2567,7 @@
         <v>67</v>
       </c>
       <c r="C24" s="10">
-        <v>0.1</v>
+        <v>0.7</v>
       </c>
       <c r="D24" s="11" t="s">
         <v>98</v>

</xml_diff>

<commit_message>
Started documenting initial configurations for Hadoop, Spark, and Kafka in "Hadoop 초기 설정.docx"
</commit_message>
<xml_diff>
--- a/WBS(WeatherBasedCareCall).xlsx
+++ b/WBS(WeatherBasedCareCall).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\art\Desktop\WeatherBasedCareCall\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{212FF7E5-68F2-4A2E-AD54-4A5D0FAA79AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E839D4B-6857-4D4E-9064-37BA2BA57024}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1021,8 +1021,8 @@
   <dimension ref="A1:AW1031"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="X22" sqref="X22"/>
+      <pane ySplit="4" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="V28" sqref="V28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2329,7 +2329,7 @@
       </c>
       <c r="C20" s="16">
         <f>AVERAGE(C21:C25)</f>
-        <v>0.74</v>
+        <v>0.8</v>
       </c>
       <c r="D20" s="11"/>
       <c r="E20" s="12"/>
@@ -2567,7 +2567,7 @@
         <v>67</v>
       </c>
       <c r="C24" s="10">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="D24" s="11" t="s">
         <v>98</v>

</xml_diff>

<commit_message>
changed project plan, and preparing another project that start from this.
</commit_message>
<xml_diff>
--- a/WBS(WeatherBasedCareCall).xlsx
+++ b/WBS(WeatherBasedCareCall).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\art\Desktop\WeatherBasedCareCall\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E839D4B-6857-4D4E-9064-37BA2BA57024}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FF8F40A-C6CF-462D-8255-1143F6394B5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -255,10 +255,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>실시간 데이터 수집 로직 개발(Kafka)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>알림 서비스 개발</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -275,26 +271,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Hadoop 초기 설정 및 연동</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>spark 초기 설정</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>spark 데이터 처리 로직 개발</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>실시간 데이터 스트리밍</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>kafka 초기 설정</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Java 애플리케이션 초기 설정</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -387,10 +367,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>실시간 데이터 처리 로직 개발 연결 및 점검(Spark, Kafka)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>이메일로 알람을 전송하는 기능 개발</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -404,6 +380,30 @@
   </si>
   <si>
     <t>유지보수 및 업데이트(미정)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hadoop 초기 설정 및 연동(제거)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>spark 초기 설정(제거)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>spark 데이터 처리 로직 개발(제거)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>실시간 데이터 수집 로직 개발(Kafka)(제거)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>실시간 데이터 처리 로직 개발 연결 및 점검(Spark, Kafka)(제거)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kafka 초기 설정(제거)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1021,8 +1021,8 @@
   <dimension ref="A1:AW1031"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V28" sqref="V28"/>
+      <pane ySplit="4" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1081,7 +1081,7 @@
     </row>
     <row r="2" spans="1:49" ht="26.25" customHeight="1">
       <c r="A2" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B2" s="44" t="s">
         <v>1</v>
@@ -1425,7 +1425,7 @@
         <v>39</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C5" s="10">
         <v>1</v>
@@ -1492,7 +1492,7 @@
         <v>0</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E6" s="12">
         <v>45219</v>
@@ -1553,7 +1553,7 @@
         <v>0</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E7" s="12">
         <v>45229</v>
@@ -1670,7 +1670,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E9" s="12">
         <v>45195</v>
@@ -1731,7 +1731,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E10" s="12">
         <v>45194</v>
@@ -1792,7 +1792,7 @@
         <v>1</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E11" s="12">
         <v>45196</v>
@@ -1909,7 +1909,7 @@
         <v>1</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E13" s="12">
         <v>45199</v>
@@ -1970,7 +1970,7 @@
         <v>1</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E14" s="12">
         <v>45200</v>
@@ -2031,7 +2031,7 @@
         <v>1</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E15" s="12">
         <v>45202</v>
@@ -2092,7 +2092,7 @@
         <v>1</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E16" s="12">
         <v>45203</v>
@@ -2153,7 +2153,7 @@
         <v>0</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E17" s="12">
         <v>45219</v>
@@ -2208,7 +2208,7 @@
     <row r="18" spans="1:49" ht="17.25" customHeight="1">
       <c r="A18" s="37"/>
       <c r="B18" s="15" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C18" s="16">
         <f>AVERAGE(C19:C19)</f>
@@ -2264,13 +2264,13 @@
     <row r="19" spans="1:49" ht="17.25" customHeight="1">
       <c r="A19" s="37"/>
       <c r="B19" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C19" s="10">
         <v>0</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E19" s="12">
         <v>45229</v>
@@ -2387,7 +2387,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E21" s="12">
         <v>45204</v>
@@ -2448,7 +2448,7 @@
         <v>1</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E22" s="12">
         <v>45205</v>
@@ -2503,13 +2503,13 @@
     <row r="23" spans="1:49" ht="17.25" customHeight="1">
       <c r="A23" s="41"/>
       <c r="B23" s="19" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
       <c r="C23" s="10">
         <v>1</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E23" s="12">
         <v>45207</v>
@@ -2570,7 +2570,7 @@
         <v>1</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E24" s="12">
         <v>45208</v>
@@ -2588,7 +2588,7 @@
       <c r="N24" s="13"/>
       <c r="O24" s="13"/>
       <c r="P24" s="13"/>
-      <c r="Q24" s="13"/>
+      <c r="Q24" s="14"/>
       <c r="R24" s="13"/>
       <c r="S24" s="13"/>
       <c r="T24" s="13"/>
@@ -2631,7 +2631,7 @@
         <v>0</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E25" s="12">
         <v>45215</v>
@@ -2742,13 +2742,13 @@
     <row r="27" spans="1:49" ht="17.25" customHeight="1">
       <c r="A27" s="41"/>
       <c r="B27" s="22" t="s">
-        <v>76</v>
+        <v>103</v>
       </c>
       <c r="C27" s="10">
         <v>0.3</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E27" s="12">
         <v>45210</v>
@@ -2803,13 +2803,13 @@
     <row r="28" spans="1:49" ht="17.25" customHeight="1">
       <c r="A28" s="41"/>
       <c r="B28" s="22" t="s">
-        <v>77</v>
+        <v>104</v>
       </c>
       <c r="C28" s="10">
         <v>0</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E28" s="12">
         <v>45211</v>
@@ -2864,13 +2864,13 @@
     <row r="29" spans="1:49" ht="17.25" customHeight="1">
       <c r="A29" s="41"/>
       <c r="B29" s="22" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C29" s="10">
         <v>0</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E29" s="12">
         <v>45214</v>
@@ -2925,11 +2925,11 @@
     <row r="30" spans="1:49" ht="17.25" customHeight="1">
       <c r="A30" s="41"/>
       <c r="B30" s="23" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C30" s="24">
         <f>AVERAGE(C31:C33)</f>
-        <v>0</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="D30" s="11"/>
       <c r="E30" s="25"/>
@@ -2981,13 +2981,13 @@
     <row r="31" spans="1:49" ht="17.25" customHeight="1">
       <c r="A31" s="41"/>
       <c r="B31" s="22" t="s">
-        <v>79</v>
+        <v>107</v>
       </c>
       <c r="C31" s="10">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E31" s="12">
         <v>45212</v>
@@ -3042,13 +3042,13 @@
     <row r="32" spans="1:49" ht="17.25" customHeight="1">
       <c r="A32" s="41"/>
       <c r="B32" s="22" t="s">
-        <v>70</v>
+        <v>105</v>
       </c>
       <c r="C32" s="10">
         <v>0</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E32" s="12">
         <v>45213</v>
@@ -3103,13 +3103,13 @@
     <row r="33" spans="1:49" ht="17.25" customHeight="1">
       <c r="A33" s="41"/>
       <c r="B33" s="26" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="C33" s="10">
         <v>0</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E33" s="12">
         <v>45214</v>
@@ -3164,7 +3164,7 @@
     <row r="34" spans="1:49" ht="17.25" customHeight="1">
       <c r="A34" s="41"/>
       <c r="B34" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C34" s="24">
         <f>AVERAGE(C35:C37)</f>
@@ -3220,13 +3220,13 @@
     <row r="35" spans="1:49" ht="17.25" customHeight="1">
       <c r="A35" s="41"/>
       <c r="B35" s="22" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C35" s="10">
         <v>0</v>
       </c>
       <c r="D35" s="11" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E35" s="12">
         <v>45216</v>
@@ -3281,13 +3281,13 @@
     <row r="36" spans="1:49" ht="17.25" customHeight="1">
       <c r="A36" s="41"/>
       <c r="B36" s="27" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C36" s="10">
         <v>0</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E36" s="12">
         <v>45220</v>
@@ -3342,13 +3342,13 @@
     <row r="37" spans="1:49" ht="17.25" customHeight="1">
       <c r="A37" s="41"/>
       <c r="B37" s="22" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C37" s="10">
         <v>0</v>
       </c>
       <c r="D37" s="11" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E37" s="12">
         <v>45222</v>
@@ -3403,7 +3403,7 @@
     <row r="38" spans="1:49" ht="17.25" customHeight="1">
       <c r="A38" s="41"/>
       <c r="B38" s="23" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C38" s="24">
         <f>AVERAGE(C39:C43)</f>
@@ -3459,13 +3459,13 @@
     <row r="39" spans="1:49" ht="17.25" customHeight="1">
       <c r="A39" s="41"/>
       <c r="B39" s="28" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C39" s="10">
         <v>0</v>
       </c>
       <c r="D39" s="11" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E39" s="12">
         <v>45224</v>
@@ -3520,13 +3520,13 @@
     <row r="40" spans="1:49" ht="17.25" customHeight="1">
       <c r="A40" s="41"/>
       <c r="B40" s="28" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C40" s="10">
         <v>0</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E40" s="12">
         <v>45225</v>
@@ -3581,13 +3581,13 @@
     <row r="41" spans="1:49" ht="17.25" customHeight="1">
       <c r="A41" s="41"/>
       <c r="B41" s="28" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C41" s="10">
         <v>0</v>
       </c>
       <c r="D41" s="11" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E41" s="12">
         <v>45225</v>
@@ -3642,13 +3642,13 @@
     <row r="42" spans="1:49" ht="17.25" customHeight="1">
       <c r="A42" s="41"/>
       <c r="B42" s="28" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C42" s="10">
         <v>0</v>
       </c>
       <c r="D42" s="11" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E42" s="12">
         <v>45226</v>
@@ -3703,13 +3703,13 @@
     <row r="43" spans="1:49" ht="17.25" customHeight="1">
       <c r="A43" s="41"/>
       <c r="B43" s="28" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C43" s="10">
         <v>0</v>
       </c>
       <c r="D43" s="11" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E43" s="12">
         <v>45226</v>
@@ -3764,7 +3764,7 @@
     <row r="44" spans="1:49" ht="17.25" customHeight="1">
       <c r="A44" s="41"/>
       <c r="B44" s="23" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C44" s="24">
         <f>AVERAGE(C45:C47)</f>
@@ -3820,13 +3820,13 @@
     <row r="45" spans="1:49" ht="17.25" customHeight="1">
       <c r="A45" s="41"/>
       <c r="B45" s="28" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C45" s="10">
         <v>0</v>
       </c>
       <c r="D45" s="11" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E45" s="12">
         <v>45227</v>
@@ -3881,13 +3881,13 @@
     <row r="46" spans="1:49" ht="17.25" customHeight="1">
       <c r="A46" s="41"/>
       <c r="B46" s="28" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C46" s="10">
         <v>0</v>
       </c>
       <c r="D46" s="11" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E46" s="12">
         <v>45227</v>
@@ -3942,13 +3942,13 @@
     <row r="47" spans="1:49" ht="17.25" customHeight="1">
       <c r="A47" s="41"/>
       <c r="B47" s="28" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C47" s="10">
         <v>0</v>
       </c>
       <c r="D47" s="11" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E47" s="12">
         <v>45227</v>
@@ -4003,7 +4003,7 @@
     <row r="48" spans="1:49" ht="17.25" customHeight="1">
       <c r="A48" s="41"/>
       <c r="B48" s="15" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C48" s="24">
         <f>AVERAGE(C49:C51)</f>
@@ -4047,7 +4047,6 @@
       <c r="AM48" s="14"/>
       <c r="AN48" s="14"/>
       <c r="AO48" s="14"/>
-      <c r="AP48" s="14"/>
       <c r="AQ48" s="14"/>
       <c r="AR48" s="14"/>
       <c r="AS48" s="14"/>
@@ -4059,13 +4058,13 @@
     <row r="49" spans="1:49" ht="17.25" customHeight="1">
       <c r="A49" s="41"/>
       <c r="B49" s="28" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C49" s="10">
         <v>0</v>
       </c>
       <c r="D49" s="11" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="E49" s="12"/>
       <c r="F49" s="12"/>
@@ -4115,7 +4114,7 @@
     <row r="50" spans="1:49" ht="17.25" customHeight="1">
       <c r="A50" s="41"/>
       <c r="B50" s="28" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C50" s="10">
         <v>0</v>
@@ -4169,7 +4168,7 @@
     <row r="51" spans="1:49" ht="17.25" customHeight="1">
       <c r="A51" s="41"/>
       <c r="B51" s="29" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C51" s="30">
         <v>0</v>
@@ -4224,7 +4223,7 @@
     <row r="52" spans="1:49" ht="17.25" customHeight="1">
       <c r="A52" s="41"/>
       <c r="B52" s="15" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="C52" s="24">
         <f>AVERAGE(C53)</f>
@@ -4280,7 +4279,7 @@
     <row r="53" spans="1:49" ht="17.25" customHeight="1">
       <c r="A53" s="41"/>
       <c r="B53" s="29" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C53" s="30">
         <v>0</v>
@@ -4335,7 +4334,7 @@
     <row r="54" spans="1:49" ht="17.25" customHeight="1">
       <c r="A54" s="41"/>
       <c r="B54" s="29" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C54" s="30">
         <v>0</v>
@@ -4390,7 +4389,7 @@
     <row r="55" spans="1:49" ht="17.25" customHeight="1">
       <c r="A55" s="41"/>
       <c r="B55" s="29" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C55" s="30">
         <v>0</v>

</xml_diff>